<commit_message>
metric124 class level data collection
</commit_message>
<xml_diff>
--- a/data analysis/Correction 1、2&6/dataAnalysisOf1&2&6.xlsx
+++ b/data analysis/Correction 1、2&6/dataAnalysisOf1&2&6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/study/master/19winter/soen6611/Metrics-Correlation-Analysis/data analysis/Correction 1、2&amp;6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE75C748-A1A4-1F4F-8142-AF2486258413}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CD9176-89D4-EB4C-8929-1147C083B28D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="1060" windowWidth="25600" windowHeight="14140" xr2:uid="{376C5903-038D-2540-A4DC-D9B9C049B8D3}"/>
+    <workbookView xWindow="8660" yWindow="7780" windowWidth="25600" windowHeight="14140" xr2:uid="{376C5903-038D-2540-A4DC-D9B9C049B8D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,66 +33,67 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>lang3.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lang3.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lang3.7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StatementCov</t>
-  </si>
-  <si>
-    <t>BranchCov</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>project</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BMI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>codec1.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>codec1.12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>collections4.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>collections4.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>configuration2.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jfreechart1.0.19</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jfreechart1.5.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>configuration2.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>configuration2.1</t>
+    <t>Total Statement Coverage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Branch Coverage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project(version)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons Lang 3.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons Lang 3.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons Lang 3.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons codec 1.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons codec 1.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons collections 4.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons collections 4.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons configuration 2.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons configuration 2.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apache commons configuration 2.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jfreechart 1.0.19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jfreechart 1.5.0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,31 +461,34 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>0.92</v>
@@ -498,7 +502,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0.95</v>
@@ -512,7 +516,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>0.95</v>
@@ -582,7 +586,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0.86</v>
@@ -596,7 +600,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.86</v>
@@ -610,7 +614,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>0.86</v>
@@ -624,7 +628,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>0.53</v>
@@ -638,7 +642,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>0.54</v>

</xml_diff>